<commit_message>
feature: enviar cartificado por email
</commit_message>
<xml_diff>
--- a/Ouvintes.xlsx
+++ b/Ouvintes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="445">
   <si>
     <t>Data: 26/08/2022</t>
   </si>
@@ -1333,16 +1333,28 @@
     <t>Dicoutosss12@gmail.com</t>
   </si>
   <si>
-    <t>Data</t>
+    <t>Email</t>
   </si>
   <si>
     <t>Pessoa 1</t>
   </si>
   <si>
+    <t>allanfernds@gmail.com</t>
+  </si>
+  <si>
     <t>Pessoa 2</t>
   </si>
   <si>
+    <t>allanweik@gmail.com</t>
+  </si>
+  <si>
     <t>Pessoa 3</t>
+  </si>
+  <si>
+    <t>alanfernandes.mm@gmail.com</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1350,7 +1362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1363,6 +1375,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -1442,13 +1460,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1457,21 +1472,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1479,6 +1497,12 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1782,129 +1806,183 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="32.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="37.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>437</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+      <c r="A2" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>439</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
-        <v>438</v>
+        <v>440</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>441</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
-        <v>439</v>
+        <v>442</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>443</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="3" t="s">
-        <v>440</v>
+      <c r="A5" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>444</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="3"/>
+      <c r="A6" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="3"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="3"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="3"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="3"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="3"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="3"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="3"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="3"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="3"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="3"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="3"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="3"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="3"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="3"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="3"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="3"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="3"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="3"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="3"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="3"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="3"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="3"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="3"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="3"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="3"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="3"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="3"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="3"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+      <c r="A36" s="11"/>
+      <c r="B36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>